<commit_message>
[ADD] New data and first optimisation models working
</commit_message>
<xml_diff>
--- a/Data/CostsData.xlsx
+++ b/Data/CostsData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://imperiallondon-my.sharepoint.com/personal/its323_ic_ac_uk/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nacho\Desktop\Imperial College\Spring Term\Power System Planning\PowerSystemPlanning_CW\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="134" documentId="8_{F7A29999-7E72-4D5C-B860-BC9BD24E616A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{379D1E75-9454-46C4-A3AF-8982DAA612CF}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50B21E6B-0A27-40EE-9BDE-587FDE42F7A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{E7D0CA2F-4CAE-422F-AE96-9629072F192C}"/>
+    <workbookView xWindow="6960" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{E7D0CA2F-4CAE-422F-AE96-9629072F192C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -80,9 +80,6 @@
     <t>Coal</t>
   </si>
   <si>
-    <t>CO2 (lb/MMBtu)</t>
-  </si>
-  <si>
     <t>Gas-CC</t>
   </si>
   <si>
@@ -96,6 +93,9 @@
   </si>
   <si>
     <t>OM $/MW-y</t>
+  </si>
+  <si>
+    <t>CO2 (kg/MMBtu)</t>
   </si>
 </sst>
 </file>
@@ -475,7 +475,7 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -499,7 +499,7 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D1" t="s">
         <v>5</v>
@@ -514,13 +514,13 @@
         <v>11</v>
       </c>
       <c r="H1" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="I1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" t="s">
         <v>18</v>
-      </c>
-      <c r="J1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.45">
@@ -786,7 +786,7 @@
         <v>2.37</v>
       </c>
       <c r="H9">
-        <v>202.3</v>
+        <v>91.761661600000011</v>
       </c>
       <c r="I9" s="2">
         <f t="shared" si="0"/>
@@ -799,7 +799,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B10">
         <v>1265</v>
@@ -820,7 +820,7 @@
         <v>1.6</v>
       </c>
       <c r="H10">
-        <v>118.6</v>
+        <v>53.796011199999995</v>
       </c>
       <c r="I10" s="2">
         <f t="shared" si="0"/>
@@ -833,7 +833,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B11">
         <v>1120</v>
@@ -854,7 +854,7 @@
         <v>1.6</v>
       </c>
       <c r="H11">
-        <v>119</v>
+        <v>53.977448000000003</v>
       </c>
       <c r="I11" s="2">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
[ADD] New generation data
</commit_message>
<xml_diff>
--- a/Data/CostsData.xlsx
+++ b/Data/CostsData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nacho\Desktop\Imperial College\Spring Term\Power System Planning\PowerSystemPlanning_CW\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50B21E6B-0A27-40EE-9BDE-587FDE42F7A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34C89E86-596B-448E-8804-E97BB9104B13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6960" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{E7D0CA2F-4CAE-422F-AE96-9629072F192C}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{E7D0CA2F-4CAE-422F-AE96-9629072F192C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -56,12 +56,6 @@
     <t>VarOM $/MWh</t>
   </si>
   <si>
-    <t>Hydro-Dam</t>
-  </si>
-  <si>
-    <t>Hydro-RoR</t>
-  </si>
-  <si>
     <t>Capacity Factor</t>
   </si>
   <si>
@@ -74,9 +68,6 @@
     <t>Fuel Cost ($/MMBtu)</t>
   </si>
   <si>
-    <t>Biomass</t>
-  </si>
-  <si>
     <t>Coal</t>
   </si>
   <si>
@@ -96,6 +87,15 @@
   </si>
   <si>
     <t>CO2 (kg/MMBtu)</t>
+  </si>
+  <si>
+    <t>Gas-CCS-95</t>
+  </si>
+  <si>
+    <t>Gas-CCS-97</t>
+  </si>
+  <si>
+    <t>Ramping</t>
   </si>
 </sst>
 </file>
@@ -134,10 +134,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -472,10 +473,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76D8C71C-5450-4A09-B565-28A32DF7A594}">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -499,28 +500,31 @@
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D1" t="s">
         <v>5</v>
       </c>
       <c r="E1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
         <v>9</v>
       </c>
-      <c r="G1" t="s">
-        <v>11</v>
-      </c>
       <c r="H1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" t="s">
         <v>19</v>
-      </c>
-      <c r="I1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.45">
@@ -556,7 +560,9 @@
         <f>C2*1000</f>
         <v>30000</v>
       </c>
-      <c r="K2" s="2"/>
+      <c r="K2" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
@@ -584,12 +590,15 @@
         <v>0</v>
       </c>
       <c r="I3" s="2">
-        <f t="shared" ref="I3:I11" si="0">PMT(5%,30,-B3*1000)</f>
+        <f t="shared" ref="I3:I10" si="0">PMT(5%,30,-B3*1000)</f>
         <v>300212.37289547641</v>
       </c>
       <c r="J3">
-        <f t="shared" ref="J3:J11" si="1">C3*1000</f>
+        <f t="shared" ref="J3:J10" si="1">C3*1000</f>
         <v>101000</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.45">
@@ -625,107 +634,120 @@
         <f t="shared" si="1"/>
         <v>23000</v>
       </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B5">
-        <v>9359</v>
+        <v>9787</v>
       </c>
       <c r="C5">
-        <v>96</v>
+        <v>135</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="E5" s="1">
-        <v>0.42</v>
+        <v>0.93</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>10.461</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <v>0.66</v>
       </c>
       <c r="H5">
         <v>0</v>
       </c>
       <c r="I5" s="2">
         <f t="shared" si="0"/>
-        <v>608816.3809163085</v>
+        <v>636658.3951306669</v>
       </c>
       <c r="J5">
         <f t="shared" si="1"/>
-        <v>96000</v>
+        <v>135000</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B6">
-        <v>7468</v>
+        <f>3549+693+2857</f>
+        <v>7099</v>
       </c>
       <c r="C6">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>8.4600000000000009</v>
       </c>
       <c r="E6" s="1">
-        <v>0.66</v>
+        <v>1</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>8.49</v>
       </c>
       <c r="G6">
-        <v>0</v>
+        <v>2.37</v>
       </c>
       <c r="H6">
-        <v>0</v>
+        <v>91.761661600000011</v>
       </c>
       <c r="I6" s="2">
         <f t="shared" si="0"/>
-        <v>485804.11717950553</v>
+        <v>461800.13763488346</v>
       </c>
       <c r="J6">
         <f t="shared" si="1"/>
-        <v>85000</v>
+        <v>78000</v>
+      </c>
+      <c r="K6">
+        <v>0.6</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B7">
-        <v>9787</v>
+        <v>1265</v>
       </c>
       <c r="C7">
-        <v>135</v>
+        <v>31</v>
       </c>
       <c r="D7">
-        <v>2.5</v>
+        <v>1.96</v>
       </c>
       <c r="E7" s="1">
-        <v>0.93</v>
+        <v>1</v>
       </c>
       <c r="F7">
-        <v>10.461</v>
+        <v>6.28</v>
       </c>
       <c r="G7">
-        <v>0.66</v>
+        <v>1.6</v>
       </c>
       <c r="H7">
-        <v>0</v>
+        <v>53.796011199999995</v>
       </c>
       <c r="I7" s="2">
         <f t="shared" si="0"/>
-        <v>636658.3951306669</v>
+        <v>82290.065376549886</v>
       </c>
       <c r="J7">
         <f t="shared" si="1"/>
-        <v>135000</v>
+        <v>31000</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.45">
@@ -733,136 +755,104 @@
         <v>12</v>
       </c>
       <c r="B8">
-        <v>5391</v>
+        <v>1120</v>
       </c>
       <c r="C8">
-        <v>157</v>
+        <v>24</v>
       </c>
       <c r="D8">
-        <v>5</v>
+        <v>6.44</v>
       </c>
       <c r="E8" s="1">
-        <v>0.64</v>
+        <v>1</v>
       </c>
       <c r="F8">
-        <v>13.5</v>
+        <v>9.7170000000000005</v>
       </c>
       <c r="G8">
-        <v>5</v>
+        <v>1.6</v>
       </c>
       <c r="H8">
-        <v>0</v>
+        <v>53.977448000000003</v>
       </c>
       <c r="I8" s="2">
         <f t="shared" si="0"/>
-        <v>350692.28651777108</v>
+        <v>72857.607289909778</v>
       </c>
       <c r="J8">
         <f t="shared" si="1"/>
-        <v>157000</v>
+        <v>24000</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B9">
-        <f>3549+693+2857</f>
-        <v>7099</v>
+        <v>2596</v>
       </c>
       <c r="C9">
-        <v>78</v>
+        <v>62</v>
       </c>
       <c r="D9">
-        <v>8.4600000000000009</v>
+        <v>4.5199999999999996</v>
       </c>
       <c r="E9" s="1">
         <v>1</v>
       </c>
       <c r="F9">
-        <v>8.49</v>
-      </c>
-      <c r="G9">
-        <v>2.37</v>
+        <v>7.11</v>
       </c>
       <c r="H9">
-        <v>91.761661600000011</v>
+        <v>5.9</v>
       </c>
       <c r="I9" s="2">
         <f t="shared" si="0"/>
-        <v>461800.13763488346</v>
+        <v>168873.525468398</v>
       </c>
       <c r="J9">
         <f t="shared" si="1"/>
-        <v>78000</v>
+        <v>62000</v>
+      </c>
+      <c r="K9">
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B10">
-        <v>1265</v>
+        <v>2635</v>
       </c>
       <c r="C10">
-        <v>31</v>
+        <v>62</v>
       </c>
       <c r="D10">
-        <v>1.96</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="E10" s="1">
         <v>1</v>
       </c>
       <c r="F10">
-        <v>6.28</v>
-      </c>
-      <c r="G10">
-        <v>1.6</v>
+        <v>7.15</v>
       </c>
       <c r="H10">
-        <v>53.796011199999995</v>
+        <v>3.6</v>
       </c>
       <c r="I10" s="2">
         <f t="shared" si="0"/>
-        <v>82290.065376549886</v>
+        <v>171410.53143652878</v>
       </c>
       <c r="J10">
         <f t="shared" si="1"/>
-        <v>31000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11">
-        <v>1120</v>
-      </c>
-      <c r="C11">
-        <v>24</v>
-      </c>
-      <c r="D11">
-        <v>6.44</v>
-      </c>
-      <c r="E11" s="1">
-        <v>1</v>
-      </c>
-      <c r="F11">
-        <v>9.7170000000000005</v>
-      </c>
-      <c r="G11">
-        <v>1.6</v>
-      </c>
-      <c r="H11">
-        <v>53.977448000000003</v>
-      </c>
-      <c r="I11" s="2">
-        <f t="shared" si="0"/>
-        <v>72857.607289909778</v>
-      </c>
-      <c r="J11">
-        <f t="shared" si="1"/>
-        <v>24000</v>
+        <v>62000</v>
+      </c>
+      <c r="K10">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[CHG] Modified costs data
</commit_message>
<xml_diff>
--- a/Data/CostsData.xlsx
+++ b/Data/CostsData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nacho\Desktop\Imperial College\Spring Term\Power System Planning\PowerSystemPlanning_CW\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34C89E86-596B-448E-8804-E97BB9104B13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65C767EF-73BC-4305-8BC3-9CCDC3EBF299}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{E7D0CA2F-4CAE-422F-AE96-9629072F192C}"/>
+    <workbookView xWindow="5910" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{E7D0CA2F-4CAE-422F-AE96-9629072F192C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Gen</t>
   </si>
@@ -96,6 +96,15 @@
   </si>
   <si>
     <t>Ramping</t>
+  </si>
+  <si>
+    <t>BESS-2H</t>
+  </si>
+  <si>
+    <t>BESS-6H</t>
+  </si>
+  <si>
+    <t>BESS-10H</t>
   </si>
 </sst>
 </file>
@@ -138,7 +147,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -473,10 +482,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76D8C71C-5450-4A09-B565-28A32DF7A594}">
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -560,7 +569,7 @@
         <f>C2*1000</f>
         <v>30000</v>
       </c>
-      <c r="K2" s="3">
+      <c r="K2">
         <v>1</v>
       </c>
     </row>
@@ -590,11 +599,11 @@
         <v>0</v>
       </c>
       <c r="I3" s="2">
-        <f t="shared" ref="I3:I10" si="0">PMT(5%,30,-B3*1000)</f>
+        <f t="shared" ref="I3:I13" si="0">PMT(5%,30,-B3*1000)</f>
         <v>300212.37289547641</v>
       </c>
       <c r="J3">
-        <f t="shared" ref="J3:J10" si="1">C3*1000</f>
+        <f t="shared" ref="J3:J13" si="1">C3*1000</f>
         <v>101000</v>
       </c>
       <c r="K3">
@@ -806,6 +815,9 @@
       <c r="F9">
         <v>7.11</v>
       </c>
+      <c r="G9">
+        <v>1.6</v>
+      </c>
       <c r="H9">
         <v>5.9</v>
       </c>
@@ -840,6 +852,9 @@
       <c r="F10">
         <v>7.15</v>
       </c>
+      <c r="G10">
+        <v>1.6</v>
+      </c>
       <c r="H10">
         <v>3.6</v>
       </c>
@@ -852,6 +867,117 @@
         <v>62000</v>
       </c>
       <c r="K10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11">
+        <v>943</v>
+      </c>
+      <c r="C11">
+        <v>24</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11" s="3">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11" s="2">
+        <f t="shared" si="0"/>
+        <v>61343.503280700817</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="1"/>
+        <v>24000</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12">
+        <v>2321</v>
+      </c>
+      <c r="C12">
+        <v>56</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12" s="2">
+        <f t="shared" si="0"/>
+        <v>150984.38082132195</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="1"/>
+        <v>56000</v>
+      </c>
+      <c r="K12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13">
+        <v>3250</v>
+      </c>
+      <c r="C13">
+        <v>88</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13" s="3">
+        <v>0.41699999999999998</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13" s="2">
+        <f t="shared" si="0"/>
+        <v>211417.16401089888</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="1"/>
+        <v>88000</v>
+      </c>
+      <c r="K13">
         <v>1</v>
       </c>
     </row>

</xml_diff>